<commit_message>
Bill of materials updated
</commit_message>
<xml_diff>
--- a/Phase 2 (Epifluorescence Microscope)/Hardware/Bill of Materials.xlsx
+++ b/Phase 2 (Epifluorescence Microscope)/Hardware/Bill of Materials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak296c\Documents\Git_Files\ModMicroUofG\Phase 2 (Epifluorescence Microscope)\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/akhil/Documents/Git Files/ModMicroUofG/Phase 2 (Epifluorescence Microscope)/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC01E66-A051-4C8B-8674-5F7B36BE0C48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2569530F-B181-424A-89CB-7C67FCECCE16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1180" yWindow="500" windowWidth="27620" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>Component/Description</t>
   </si>
@@ -228,6 +228,51 @@
   </si>
   <si>
     <t>USB cable, Required: 1</t>
+  </si>
+  <si>
+    <t>Pozi Pan Self Tapping Screw (AB) No.2 x 6.5mm in A2 Stainless - DIN 7981 (pack of 40)</t>
+  </si>
+  <si>
+    <t>https://www.westfieldfasteners.co.uk/Self-Tapping-Screws/Pozi-Pan-Self-Tapping-Screw-AB-No.2x6.5-A2-Stainless.html</t>
+  </si>
+  <si>
+    <t>C1RC/M - Slip Ring for Ø1" (Ø25.4 mm) Components, M4 Tap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.thorlabs.com/thorproduct.cfm?partnumber=C1RC/M </t>
+  </si>
+  <si>
+    <t>TR50/M - Ø12.7 mm Optical Post, SS, M4 Setscrew, M6 Tap, L = 50 mm</t>
+  </si>
+  <si>
+    <t>PH1.5E - Ø1/2" Pedestal Post Holder, Spring-Loaded Hex-Locking Thumbscrew, L=1.69"</t>
+  </si>
+  <si>
+    <t>https://www.thorlabs.com/thorproduct.cfm?partnumber=TR50/M</t>
+  </si>
+  <si>
+    <t>https://www.thorlabs.com/thorproduct.cfm?partnumber=PH1.5E#ad-image-0</t>
+  </si>
+  <si>
+    <t>M2.2x6.5 mm self tapping screws, Required: 2</t>
+  </si>
+  <si>
+    <t>1" Slip Ring, Required: 1</t>
+  </si>
+  <si>
+    <t>Optical Post, Required: 1</t>
+  </si>
+  <si>
+    <t>Pedestal Post Holder, Required: 1</t>
+  </si>
+  <si>
+    <t>optical PMMA plano convex lens diameter 13mm focal length 5mm (Pack of 100)</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/w/wholesale-13mm-5mm-pmma-lens.html</t>
+  </si>
+  <si>
+    <t>Condenser Lens, Required: 2</t>
   </si>
 </sst>
 </file>
@@ -235,12 +280,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
-    <numFmt numFmtId="168" formatCode="&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -259,6 +311,15 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -266,33 +327,12 @@
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -324,7 +364,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -347,41 +387,62 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -699,149 +760,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.28515625" customWidth="1"/>
-    <col min="2" max="2" width="86.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
-    <col min="6" max="6" width="136.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.33203125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="86.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="11" customWidth="1"/>
+    <col min="6" max="6" width="136.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7" ht="120" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="20" t="s">
+      <c r="C1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="8">
-        <v>1</v>
-      </c>
-      <c r="D2" s="10">
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
         <v>13.33</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="3">
         <f>D2*C2</f>
         <v>13.33</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="8">
-        <v>1</v>
-      </c>
-      <c r="D3" s="10">
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3">
         <v>4.0599999999999996</v>
       </c>
-      <c r="E3" s="10">
-        <f t="shared" ref="E3:E8" si="0">D3*C3</f>
+      <c r="E3" s="3">
+        <f t="shared" ref="E3:E9" si="0">D3*C3</f>
         <v>4.0599999999999996</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="8">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10">
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3">
         <v>1.4</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="3">
         <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="8">
-        <v>1</v>
-      </c>
-      <c r="D5" s="10">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="3">
         <v>1.31</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="3">
         <f t="shared" si="0"/>
         <v>1.31</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="8">
-        <v>1</v>
-      </c>
-      <c r="D6" s="9">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="12">
         <v>4.99</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="3">
         <f t="shared" si="0"/>
         <v>4.99</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
         <v>53</v>
       </c>
@@ -854,313 +916,423 @@
       <c r="D7" s="14">
         <v>9.08</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="3">
         <f t="shared" si="0"/>
         <v>9.08</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="10">
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
         <v>32.5</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="3">
         <f t="shared" si="0"/>
         <v>32.5</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="2">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2.12</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>2.12</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B11" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="13">
-        <v>1</v>
-      </c>
-      <c r="D10" s="14">
+      <c r="C11" s="13">
+        <v>1</v>
+      </c>
+      <c r="D11" s="14">
         <v>308.63</v>
       </c>
-      <c r="E10" s="14">
-        <f>D10*C10</f>
+      <c r="E11" s="14">
+        <f>D11*C11</f>
         <v>308.63</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F11" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="13">
-        <v>1</v>
-      </c>
-      <c r="D11" s="14">
+      <c r="C12" s="13">
+        <v>1</v>
+      </c>
+      <c r="D12" s="14">
         <v>205.27</v>
       </c>
-      <c r="E11" s="14">
-        <f t="shared" ref="E11:E14" si="1">D11*C11</f>
+      <c r="E12" s="14">
+        <f t="shared" ref="E12:E16" si="1">D12*C12</f>
         <v>205.27</v>
       </c>
-      <c r="F11" s="11" t="s">
+      <c r="F12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="13">
-        <v>1</v>
-      </c>
-      <c r="D12" s="14">
+      <c r="C13" s="13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="14">
         <v>207.89</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E13" s="14">
         <f t="shared" si="1"/>
         <v>207.89</v>
       </c>
-      <c r="F12" s="11" t="s">
+      <c r="F13" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B14" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="14">
+      <c r="C14" s="13">
+        <v>1</v>
+      </c>
+      <c r="D14" s="14">
         <v>65.510000000000005</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E14" s="14">
         <f t="shared" si="1"/>
         <v>65.510000000000005</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="F14" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" s="13">
+        <v>1</v>
+      </c>
+      <c r="D15" s="14">
+        <v>21.78</v>
+      </c>
+      <c r="E15" s="14">
+        <f t="shared" si="1"/>
+        <v>21.78</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="13">
-        <v>1</v>
-      </c>
-      <c r="D14" s="14">
+      <c r="C16" s="13">
+        <v>1</v>
+      </c>
+      <c r="D16" s="14">
         <v>21.25</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E16" s="14">
         <f t="shared" si="1"/>
         <v>21.25</v>
       </c>
-      <c r="F14" s="11" t="s">
+      <c r="F16" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-    </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B16" s="16" t="s">
+      <c r="B18" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="8">
-        <v>1</v>
-      </c>
-      <c r="D16" s="10">
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3">
         <v>36.64</v>
       </c>
-      <c r="E16" s="10">
-        <f>D16*C16</f>
+      <c r="E18" s="3">
+        <f>D18*C18</f>
         <v>36.64</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F18" s="8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B17" s="16" t="s">
+      <c r="B19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="8">
-        <v>1</v>
-      </c>
-      <c r="D17" s="10">
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
+      <c r="D19" s="3">
         <v>7.04</v>
       </c>
-      <c r="E17" s="10">
-        <f t="shared" ref="E17:E21" si="2">D17*C17</f>
+      <c r="E19" s="3">
+        <f t="shared" ref="E19:E23" si="2">D19*C19</f>
         <v>7.04</v>
       </c>
-      <c r="F17" s="17" t="s">
+      <c r="F19" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B18" s="16" t="s">
+      <c r="B20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="8">
-        <v>1</v>
-      </c>
-      <c r="D18" s="10">
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
         <v>22</v>
       </c>
-      <c r="E18" s="10">
+      <c r="E20" s="3">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F20" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="8">
-        <v>1</v>
-      </c>
-      <c r="D19" s="10">
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
         <v>5.79</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E21" s="3">
         <f t="shared" si="2"/>
         <v>5.79</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F21" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B22" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="8">
-        <v>1</v>
-      </c>
-      <c r="D20" s="10">
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3">
         <v>2.1800000000000002</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E22" s="3">
         <f t="shared" si="2"/>
         <v>2.1800000000000002</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F22" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="15" t="s">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B23" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="8">
-        <v>1</v>
-      </c>
-      <c r="D21" s="10">
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3">
         <v>17.989999999999998</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E23" s="3">
         <f t="shared" si="2"/>
         <v>17.989999999999998</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F23" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="9">
+        <v>1</v>
+      </c>
+      <c r="D25" s="16">
+        <v>22.27</v>
+      </c>
+      <c r="E25" s="16">
+        <v>22.27</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="9">
+        <v>1</v>
+      </c>
+      <c r="D26" s="10">
+        <v>4.43</v>
+      </c>
+      <c r="E26" s="16">
+        <v>4.43</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="9">
+        <v>1</v>
+      </c>
+      <c r="D27" s="16">
+        <v>20.53</v>
+      </c>
+      <c r="E27" s="16">
+        <v>20.53</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="B32" s="19"/>
+    </row>
+    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="3"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B34" s="19"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="17" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1169,26 +1341,30 @@
     <hyperlink ref="F3" r:id="rId1" xr:uid="{EE1231C2-0066-40F4-8230-0E87D4E86458}"/>
     <hyperlink ref="F4" r:id="rId2" xr:uid="{B5C87DB9-67A3-4B43-8219-C3DFB8BE3E18}"/>
     <hyperlink ref="F5" r:id="rId3" xr:uid="{57C6979A-845E-443D-8396-760B43C332FA}"/>
-    <hyperlink ref="F16" r:id="rId4" xr:uid="{C30F9A40-7F5B-452A-BEC1-5E9D085DEA12}"/>
-    <hyperlink ref="F17" r:id="rId5" xr:uid="{AF19FBAC-7122-4255-A00A-7C7FBDDFB816}"/>
-    <hyperlink ref="F18" r:id="rId6" display="https://uk.farnell.com/raspberry-pi/rpi-8mp-camera-board/raspberry-pi-camera-board-v2/dp/3677845?CMP=KNC-GUK-GEN-KWL-CLM-CARTABAN-10OFF&amp;mckv=_dc|pcrid|626593324211|kword||match||plid||slid||product||pgrid|140532649805|ptaid|aud-140011313109:dsa-1814079156442|&amp;gclid=CjwKCAjwov6hBhBsEiwAvrvN6O-aklIc29pCxqZq4iy2P648nNDc3e5c-JIW7EuwekTS0EeazyuRuRoCW4YQAvD_BwE" xr:uid="{D97F6DEB-3769-488B-8D2D-49B2CBA54924}"/>
-    <hyperlink ref="F19" r:id="rId7" xr:uid="{23D8DDE1-9C39-4A94-8346-1A562048FF58}"/>
-    <hyperlink ref="F20" r:id="rId8" xr:uid="{B9C4FEC3-F4C4-4198-B471-E695CE5C2E42}"/>
-    <hyperlink ref="F21" r:id="rId9" xr:uid="{62435716-4663-4AC3-A5BB-F87BF7A90CB0}"/>
-    <hyperlink ref="A27" r:id="rId10" xr:uid="{0765AC03-B52E-4DEF-B0C3-FE22DF19B88F}"/>
-    <hyperlink ref="A29" r:id="rId11" xr:uid="{AC84DA97-25AE-4326-B1DC-13726780FE3A}"/>
+    <hyperlink ref="F18" r:id="rId4" xr:uid="{C30F9A40-7F5B-452A-BEC1-5E9D085DEA12}"/>
+    <hyperlink ref="F19" r:id="rId5" xr:uid="{AF19FBAC-7122-4255-A00A-7C7FBDDFB816}"/>
+    <hyperlink ref="F20" r:id="rId6" display="https://uk.farnell.com/raspberry-pi/rpi-8mp-camera-board/raspberry-pi-camera-board-v2/dp/3677845?CMP=KNC-GUK-GEN-KWL-CLM-CARTABAN-10OFF&amp;mckv=_dc|pcrid|626593324211|kword||match||plid||slid||product||pgrid|140532649805|ptaid|aud-140011313109:dsa-1814079156442|&amp;gclid=CjwKCAjwov6hBhBsEiwAvrvN6O-aklIc29pCxqZq4iy2P648nNDc3e5c-JIW7EuwekTS0EeazyuRuRoCW4YQAvD_BwE" xr:uid="{D97F6DEB-3769-488B-8D2D-49B2CBA54924}"/>
+    <hyperlink ref="F21" r:id="rId7" xr:uid="{23D8DDE1-9C39-4A94-8346-1A562048FF58}"/>
+    <hyperlink ref="F22" r:id="rId8" xr:uid="{B9C4FEC3-F4C4-4198-B471-E695CE5C2E42}"/>
+    <hyperlink ref="F23" r:id="rId9" xr:uid="{62435716-4663-4AC3-A5BB-F87BF7A90CB0}"/>
+    <hyperlink ref="A32" r:id="rId10" xr:uid="{0765AC03-B52E-4DEF-B0C3-FE22DF19B88F}"/>
+    <hyperlink ref="A34" r:id="rId11" xr:uid="{AC84DA97-25AE-4326-B1DC-13726780FE3A}"/>
     <hyperlink ref="F8" r:id="rId12" xr:uid="{26C3EC74-AD28-4887-84D8-8DA878898D3C}"/>
     <hyperlink ref="F7" r:id="rId13" xr:uid="{639C0441-3620-4E85-AD4A-5D7E90CD2C86}"/>
-    <hyperlink ref="F10" r:id="rId14" xr:uid="{40702B0E-E730-4769-A692-501C4B4C7F70}"/>
-    <hyperlink ref="F14" r:id="rId15" xr:uid="{339CE24C-D9BC-47F1-8170-F9EF8990E7D9}"/>
-    <hyperlink ref="F13" r:id="rId16" xr:uid="{843CF70C-0A3E-4671-A174-25E4C721DD28}"/>
-    <hyperlink ref="A32" r:id="rId17" xr:uid="{D1AC2E77-E333-47A9-BEE8-9F19086F6B16}"/>
-    <hyperlink ref="F11" r:id="rId18" xr:uid="{C5D98E4B-64C9-483E-933A-3997106FC769}"/>
-    <hyperlink ref="F12" r:id="rId19" xr:uid="{82067098-1FE1-4A47-A229-B832F1E0A76C}"/>
+    <hyperlink ref="F11" r:id="rId14" xr:uid="{40702B0E-E730-4769-A692-501C4B4C7F70}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{339CE24C-D9BC-47F1-8170-F9EF8990E7D9}"/>
+    <hyperlink ref="F14" r:id="rId16" xr:uid="{843CF70C-0A3E-4671-A174-25E4C721DD28}"/>
+    <hyperlink ref="A37" r:id="rId17" xr:uid="{D1AC2E77-E333-47A9-BEE8-9F19086F6B16}"/>
+    <hyperlink ref="F12" r:id="rId18" xr:uid="{C5D98E4B-64C9-483E-933A-3997106FC769}"/>
+    <hyperlink ref="F13" r:id="rId19" xr:uid="{82067098-1FE1-4A47-A229-B832F1E0A76C}"/>
     <hyperlink ref="F2" r:id="rId20" xr:uid="{AB511339-1BA9-462E-8D80-9B1C9932AB31}"/>
     <hyperlink ref="F6" r:id="rId21" xr:uid="{3E555C6A-7493-4D9B-B9F7-7AA2D1A3409C}"/>
+    <hyperlink ref="F25" r:id="rId22" xr:uid="{6597C476-F2B7-4366-9F75-79C78C499DBE}"/>
+    <hyperlink ref="F26" r:id="rId23" xr:uid="{49461C15-3D2E-4313-9743-368E08CE1BFD}"/>
+    <hyperlink ref="F27" r:id="rId24" location="ad-image-0" xr:uid="{B0A4464A-40A8-4DFD-B670-40B868DB385F}"/>
+    <hyperlink ref="F15" r:id="rId25" xr:uid="{D7C38ED0-2B2F-4647-B6FD-8E02D94A1573}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>